<commit_message>
Latest Code After Merge
</commit_message>
<xml_diff>
--- a/Data/DataView_SK_REG - SMOKE TEST3.xlsx
+++ b/Data/DataView_SK_REG - SMOKE TEST3.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551F1BC7-E876-4517-87CC-E6B09ECA5E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -176,29 +175,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color rgb="FF9CDCFE"/>
+      <family val="3"/>
       <sz val="11"/>
-      <color rgb="FF9CDCFE"/>
       <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -575,14 +574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.1796875" customWidth="1"/>
     <col min="2" max="2" width="32.81640625" customWidth="1"/>
@@ -592,7 +591,7 @@
     <col min="6" max="6" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="14.5" customHeight="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -609,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10648949</v>
       </c>
@@ -626,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10648949</v>
       </c>
@@ -643,7 +642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10648949</v>
       </c>
@@ -660,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10648949</v>
       </c>
@@ -677,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10648949</v>
       </c>
@@ -694,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10648949</v>
       </c>
@@ -711,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10648949</v>
       </c>
@@ -728,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10648949</v>
       </c>
@@ -745,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10648949</v>
       </c>
@@ -762,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10648949</v>
       </c>
@@ -779,7 +778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10648949</v>
       </c>
@@ -796,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10648949</v>
       </c>
@@ -813,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10648949</v>
       </c>
@@ -830,7 +829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10648949</v>
       </c>
@@ -847,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10648949</v>
       </c>
@@ -864,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10648949</v>
       </c>
@@ -881,7 +880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10648949</v>
       </c>
@@ -898,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10648949</v>
       </c>
@@ -915,7 +914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10648949</v>
       </c>
@@ -932,7 +931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10648949</v>
       </c>
@@ -949,7 +948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10648949</v>
       </c>
@@ -966,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10648949</v>
       </c>
@@ -983,7 +982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10648949</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10648949</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10648949</v>
       </c>
@@ -1034,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10648949</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10648949</v>
       </c>
@@ -1068,7 +1067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10648949</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10648949</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10648949</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10648949</v>
       </c>
@@ -1136,7 +1135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10648949</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10648949</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10648949</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10648949</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10648949</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10648949</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10648949</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>10648949</v>
       </c>
@@ -1272,7 +1271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10648949</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" ht="15.65" customHeight="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>10648995</v>
       </c>
@@ -1300,7 +1299,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>10648995</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>10648995</v>
       </c>
@@ -1322,7 +1321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>10648995</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>10648995</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>10648995</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>10648995</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>10648995</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>10648995</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>10648995</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>10648995</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>10648995</v>
       </c>
@@ -1421,7 +1420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>10648995</v>
       </c>
@@ -1432,7 +1431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>10648995</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>10648995</v>
       </c>
@@ -1454,7 +1453,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>10648995</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>10648995</v>
       </c>
@@ -1476,7 +1475,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>10648995</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>10648995</v>
       </c>
@@ -1498,7 +1497,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>10648995</v>
       </c>
@@ -1509,7 +1508,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>10648995</v>
       </c>
@@ -1520,7 +1519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>10648995</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>10648995</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>10648995</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>10648995</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>10648995</v>
       </c>
@@ -1575,7 +1574,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>10648995</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>10648995</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>10648995</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>10648995</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>10648995</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>10648995</v>
       </c>
@@ -1641,7 +1640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>10648995</v>
       </c>
@@ -1652,7 +1651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>10648995</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>10648995</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>10648995</v>
       </c>
@@ -1685,7 +1684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>10648995</v>
       </c>
@@ -1696,7 +1695,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>10648995</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>10648995</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>10648995</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" ht="15.65" customHeight="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>10648785</v>
       </c>
@@ -1746,7 +1745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>10648785</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>10648785</v>
       </c>
@@ -1780,7 +1779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>10648785</v>
       </c>
@@ -1797,7 +1796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>10648785</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>10648785</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>10648785</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>10648785</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>10648785</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>10648785</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>10648785</v>
       </c>
@@ -1916,7 +1915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>10648785</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>10648785</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>10648785</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>10648785</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>10648785</v>
       </c>
@@ -2001,7 +2000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>10648785</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>10648785</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>10648785</v>
       </c>
@@ -2052,7 +2051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10648785</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>10648785</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>10648785</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>10648785</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>10648785</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>10648785</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>10648785</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>10648785</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>10648785</v>
       </c>
@@ -2205,7 +2204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>10648785</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>10648785</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>10648785</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>10648785</v>
       </c>
@@ -2273,7 +2272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>10648785</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>10648785</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>10648785</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>10648785</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>10648785</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>10648785</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>10648785</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>10648785</v>
       </c>
@@ -2411,6 +2410,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
latest Code for Dataview Testcase
</commit_message>
<xml_diff>
--- a/Data/DataView_SK_REG - SMOKE TEST3.xlsx
+++ b/Data/DataView_SK_REG - SMOKE TEST3.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551F1BC7-E876-4517-87CC-E6B09ECA5E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -175,29 +176,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
       <family val="3"/>
-      <sz val="11"/>
-      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="2">
@@ -574,14 +575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.65" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.1796875" customWidth="1"/>
     <col min="2" max="2" width="32.81640625" customWidth="1"/>
@@ -591,7 +592,7 @@
     <col min="6" max="6" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" customHeight="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10648949</v>
       </c>
@@ -625,7 +626,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10648949</v>
       </c>
@@ -642,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10648949</v>
       </c>
@@ -659,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10648949</v>
       </c>
@@ -676,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10648949</v>
       </c>
@@ -693,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10648949</v>
       </c>
@@ -710,7 +711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10648949</v>
       </c>
@@ -727,7 +728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10648949</v>
       </c>
@@ -744,7 +745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10648949</v>
       </c>
@@ -761,7 +762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10648949</v>
       </c>
@@ -778,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10648949</v>
       </c>
@@ -795,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10648949</v>
       </c>
@@ -812,7 +813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10648949</v>
       </c>
@@ -829,7 +830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10648949</v>
       </c>
@@ -846,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10648949</v>
       </c>
@@ -863,7 +864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10648949</v>
       </c>
@@ -880,7 +881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10648949</v>
       </c>
@@ -897,7 +898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10648949</v>
       </c>
@@ -914,7 +915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10648949</v>
       </c>
@@ -931,7 +932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10648949</v>
       </c>
@@ -948,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10648949</v>
       </c>
@@ -965,7 +966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10648949</v>
       </c>
@@ -982,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10648949</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>10648949</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>10648949</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10648949</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>10648949</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>10648949</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>10648949</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10648949</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>10648949</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>10648949</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>10648949</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>10648949</v>
       </c>
@@ -1186,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>10648949</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>10648949</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>10648949</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>10648949</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>10648949</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" ht="14.5" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>10648949</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" ht="15.65" customHeight="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>10648995</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>10648995</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>10648995</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>10648995</v>
       </c>
@@ -1332,7 +1333,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>10648995</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>10648995</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>10648995</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>10648995</v>
       </c>
@@ -1376,7 +1377,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>10648995</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>10648995</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>10648995</v>
       </c>
@@ -1409,7 +1410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>10648995</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>10648995</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>10648995</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>10648995</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>10648995</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>10648995</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>10648995</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>10648995</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="61" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>10648995</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>10648995</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>10648995</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>10648995</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>10648995</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>10648995</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>10648995</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>10648995</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>10648995</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>10648995</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>10648995</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="72" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>10648995</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>10648995</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>10648995</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>10648995</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>10648995</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="77" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>10648995</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>10648995</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="79" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>10648995</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>10648995</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>10648995</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" ht="15.65" customHeight="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>10648785</v>
       </c>
@@ -1745,7 +1746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>10648785</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>10648785</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>10648785</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>10648785</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>10648785</v>
       </c>
@@ -1830,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>10648785</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>10648785</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>10648785</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>10648785</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>10648785</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>10648785</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>10648785</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>10648785</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>10648785</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>10648785</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>10648785</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>10648785</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>10648785</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>10648785</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>10648785</v>
       </c>
@@ -2085,7 +2086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>10648785</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>10648785</v>
       </c>
@@ -2119,7 +2120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>10648785</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>10648785</v>
       </c>
@@ -2153,7 +2154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>10648785</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>10648785</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>10648785</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>10648785</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>10648785</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>10648785</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>10648785</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>10648785</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>10648785</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>10648785</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>10648785</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>10648785</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>10648785</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>10648785</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" ht="15.65" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>10648785</v>
       </c>
@@ -2410,6 +2411,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>